<commit_message>
update on webpage since last time
</commit_message>
<xml_diff>
--- a/Risks.xlsx
+++ b/Risks.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68f9195abb248b09/Desktop/Fürs Studium/6 LLM as a tool for behavioral research/Code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_C154E9045B443E4078DF49B7CC2528E350C24297" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AFA415F-2DCF-4043-A791-E78AF0346A58}"/>
+  <bookViews>
+    <workbookView xWindow="15240" yWindow="975" windowWidth="33690" windowHeight="17895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -577,35 +586,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -615,7 +628,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -637,56 +650,46 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -876,27 +879,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.88"/>
-    <col customWidth="1" min="3" max="3" width="18.75"/>
-    <col customWidth="1" min="4" max="4" width="17.38"/>
-    <col customWidth="1" min="5" max="5" width="16.25"/>
-    <col customWidth="1" min="6" max="6" width="22.0"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,9 +933,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -948,9 +956,9 @@
       <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="L2" s="6" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="L2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -963,9 +971,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -982,28 +990,28 @@
       <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="L3" s="6" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="L3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>29</v>
@@ -1020,28 +1028,28 @@
       <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="L4" s="6" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>39</v>
@@ -1058,28 +1066,28 @@
       <c r="F5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="L5" s="6" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -1099,10 +1107,10 @@
       <c r="H6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>55</v>
       </c>
       <c r="N6" s="2" t="s">
@@ -1112,9 +1120,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>58</v>
@@ -1144,9 +1152,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>67</v>
@@ -1163,19 +1171,19 @@
       <c r="F8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>75</v>
@@ -1192,19 +1200,19 @@
       <c r="F9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>82</v>
@@ -1218,19 +1226,19 @@
       <c r="E10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>89</v>
@@ -1250,13 +1258,13 @@
       <c r="M11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>96</v>
@@ -1273,16 +1281,16 @@
       <c r="F12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>101</v>
@@ -1302,13 +1310,13 @@
       <c r="M13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>107</v>
@@ -1328,13 +1336,13 @@
       <c r="M14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>113</v>
@@ -1355,9 +1363,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>118</v>
@@ -1378,9 +1386,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>124</v>
@@ -1397,13 +1405,13 @@
       <c r="F17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>128</v>
@@ -1424,9 +1432,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>133</v>
@@ -1443,13 +1451,13 @@
       <c r="F19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>137</v>
@@ -1467,9 +1475,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>141</v>
@@ -1487,7 +1495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>145</v>
       </c>
@@ -1501,7 +1509,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>149</v>
       </c>
@@ -1515,7 +1523,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>153</v>
       </c>
@@ -1529,7 +1537,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>157</v>
       </c>
@@ -1543,7 +1551,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>161</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>165</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>169</v>
       </c>
@@ -1579,7 +1587,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>171</v>
       </c>
@@ -1590,7 +1598,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
         <v>174</v>
       </c>
@@ -1598,7 +1606,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
         <v>164</v>
       </c>
@@ -1606,7 +1614,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
         <v>177</v>
       </c>
@@ -1614,7 +1622,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
         <v>179</v>
       </c>
@@ -1622,8 +1630,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="9"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
       <c r="C39" s="2" t="s">
         <v>181</v>
       </c>
@@ -1631,17 +1639,17 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
         <v>184</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>